<commit_message>
feat: Program reads from excel file
The program now reads rows from the excel file which stores the data of high scores. Currently the data is only printed to the output. This was just to check if it works correctly and I will be working on displaying it to the TableView in the start screen.
</commit_message>
<xml_diff>
--- a/out/production/CW - Snake/Application/SnakeeLeaderboard.xlsx
+++ b/out/production/CW - Snake/Application/SnakeeLeaderboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8800a6e080b81c6/Documents/University/Computer Science/Year 2/COMP2013 - Developing Maintainable Software/CW - Snake/src/Application/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{16BD9B3F-2731-4BB7-9ABF-FAB864AEE52E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{16BD9B3F-2731-4BB7-9ABF-FAB864AEE52E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4A82035-61BA-41BD-BBDA-EAAF175D6667}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D40E3BD0-85A9-41B2-A0C0-5D47A818CA67}"/>
   </bookViews>
@@ -44,10 +44,10 @@
     <t>Score</t>
   </si>
   <si>
-    <t>Difficulty</t>
+    <t>Jack</t>
   </si>
   <si>
-    <t>Bombs on?</t>
+    <t>Jack Better</t>
   </si>
 </sst>
 </file>
@@ -100,6 +100,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -399,29 +403,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9215E21-896C-4D65-A0C5-9F11F4286E77}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
+      <c r="B3">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B3">
+    <sortCondition descending="1" ref="B2:B3"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Data added to excel file after game has ended
When the game ends, the player name and score from that round is added to the File and will be displayed in the leaderboard.

I have also added different leaderboards, based on whether bombs were active and the difficulty selected.
</commit_message>
<xml_diff>
--- a/out/production/CW - Snake/Application/SnakeeLeaderboard.xlsx
+++ b/out/production/CW - Snake/Application/SnakeeLeaderboard.xlsx
@@ -3,21 +3,26 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8800a6e080b81c6/Documents/University/Computer Science/Year 2/COMP2013 - Developing Maintainable Software/CW - Snake/src/Application/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{16BD9B3F-2731-4BB7-9ABF-FAB864AEE52E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4A82035-61BA-41BD-BBDA-EAAF175D6667}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="8_{16BD9B3F-2731-4BB7-9ABF-FAB864AEE52E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0578DC02-7B7F-4F69-92E9-231457EBA0ED}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D40E3BD0-85A9-41B2-A0C0-5D47A818CA67}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{D40E3BD0-85A9-41B2-A0C0-5D47A818CA67}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="3">
   <si>
     <t>Name</t>
   </si>
@@ -44,16 +49,14 @@
     <t>Score</t>
   </si>
   <si>
-    <t>Jack</t>
-  </si>
-  <si>
-    <t>Jack Better</t>
+    <t>test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -100,10 +103,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -402,43 +401,233 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9215E21-896C-4D65-A0C5-9F11F4286E77}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD05B22-988A-4146-BED8-42077AB0D08E}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n" s="0">
+        <v>521.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0"/>
+      <c r="B4" t="n" s="0">
+        <v>521.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B939D878-E8C6-4A7A-8E0A-E08F83168427}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B2" t="n" s="0">
+        <v>521.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98060BC9-2618-4D68-A88C-007ABEB60946}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n" s="0">
+        <v>521.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E3FC53-DF6F-45BF-A277-ACA82C20E2D9}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n" s="0">
+        <v>521.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F06A1B3-4662-4CB9-A146-4F17B36F623F}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n" s="0">
+        <v>2605.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6348C88F-41BF-45E4-838C-56BA43C0AFD0}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0">
         <v>5</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B3">
-    <sortCondition descending="1" ref="B2:B3"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
bug: User was able to play without entering a name first
User could start the game without entering a name, causing the leaderboard to store the score but have a blank at the name, this has now been fixed
</commit_message>
<xml_diff>
--- a/out/production/CW - Snake/Application/SnakeeLeaderboard.xlsx
+++ b/out/production/CW - Snake/Application/SnakeeLeaderboard.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="4">
   <si>
     <t>Name</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>Jack</t>
   </si>
 </sst>
 </file>
@@ -402,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD05B22-988A-4146-BED8-42077AB0D08E}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -438,6 +441,14 @@
       <c r="A4" s="0"/>
       <c r="B4" t="n" s="0">
         <v>521.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n" s="0">
+        <v>1042.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Added walls to the game
If the wall is hit, the snake loses a body part and score. If the snake is just a head and it hits the wall, the game ends.
</commit_message>
<xml_diff>
--- a/out/production/CW - Snake/Application/SnakeeLeaderboard.xlsx
+++ b/out/production/CW - Snake/Application/SnakeeLeaderboard.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -53,6 +53,18 @@
   </si>
   <si>
     <t>Jack</t>
+  </si>
+  <si>
+    <t>jg</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>jh</t>
+  </si>
+  <si>
+    <t>jk</t>
   </si>
 </sst>
 </file>
@@ -405,7 +417,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD05B22-988A-4146-BED8-42077AB0D08E}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -449,6 +461,78 @@
       </c>
       <c r="B5" t="n" s="0">
         <v>1042.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B6" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B7" t="n" s="0">
+        <v>2084.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B8" t="n" s="0">
+        <v>1042.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B9" t="n" s="0">
+        <v>3647.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B10" t="n" s="0">
+        <v>521.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B11" t="n" s="0">
+        <v>521.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B12" t="n" s="0">
+        <v>521.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B13" t="n" s="0">
+        <v>4689.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B14" t="n" s="0">
+        <v>4689.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: Created some new function for duplicate code
Any code that was often duplicated, I created a function for.

For example, there was a few times where the code created bounds and then checked if the snake head intersected with these bounds. I put this into a function CheckBounds where a Node is sent and the function checks if the snakehead intersects with the given Node.
</commit_message>
<xml_diff>
--- a/out/production/CW - Snake/Application/SnakeeLeaderboard.xlsx
+++ b/out/production/CW - Snake/Application/SnakeeLeaderboard.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>jk</t>
+  </si>
+  <si>
+    <t>j</t>
   </si>
 </sst>
 </file>
@@ -417,7 +420,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD05B22-988A-4146-BED8-42077AB0D08E}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -533,6 +536,14 @@
       </c>
       <c r="B14" t="n" s="0">
         <v>4689.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B15" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -612,7 +623,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E3FC53-DF6F-45BF-A277-ACA82C20E2D9}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -642,6 +653,14 @@
       </c>
       <c r="B3" t="n" s="0">
         <v>521.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B4" t="n" s="0">
+        <v>2084.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: User can now move the snake with WASD
User can now move the snake with both WASD and the arrow keys
</commit_message>
<xml_diff>
--- a/out/production/CW - Snake/Application/SnakeeLeaderboard.xlsx
+++ b/out/production/CW - Snake/Application/SnakeeLeaderboard.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>j</t>
+  </si>
+  <si>
+    <t>l7</t>
   </si>
 </sst>
 </file>
@@ -709,7 +712,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6348C88F-41BF-45E4-838C-56BA43C0AFD0}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
@@ -741,6 +744,14 @@
         <v>1042.0</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
chore: Removed any unused imports and variables
</commit_message>
<xml_diff>
--- a/out/production/CW - Snake/Application/SnakeeLeaderboard.xlsx
+++ b/out/production/CW - Snake/Application/SnakeeLeaderboard.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -556,7 +556,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B939D878-E8C6-4A7A-8E0A-E08F83168427}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -578,6 +578,14 @@
       </c>
       <c r="B2" t="n" s="0">
         <v>521.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B3" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: Wall sometimes spawned half out of bounds
</commit_message>
<xml_diff>
--- a/out/production/CW - Snake/Application/SnakeeLeaderboard.xlsx
+++ b/out/production/CW - Snake/Application/SnakeeLeaderboard.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -423,7 +423,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD05B22-988A-4146-BED8-42077AB0D08E}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -547,6 +547,14 @@
       </c>
       <c r="B15" t="n" s="0">
         <v>0.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B16" t="n" s="0">
+        <v>9378.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>